<commit_message>
fix AC finish bug
</commit_message>
<xml_diff>
--- a/doc/PC与PLC通信协议20170320-back.xlsx
+++ b/doc/PC与PLC通信协议20170320-back.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17830"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mywork\softproject\170215yidaRobot\doc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23895" windowHeight="10350"/>
+    <workbookView windowWidth="23895" windowHeight="10350"/>
   </bookViews>
   <sheets>
     <sheet name="B区PC与PLC通信OPC变量" sheetId="2" r:id="rId1"/>
@@ -20,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294">
   <si>
     <t>B区PC与PLC通信OPC变量</t>
   </si>
@@ -904,37 +899,19 @@
   </si>
   <si>
     <t>MicroWin.S7-1200.NewItem133</t>
-  </si>
-  <si>
-    <t>MicroWin.S7-1200.NewItem86</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>机器人状态可以直接从机器人电柜里接信号</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>称重</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>称重</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>称重标签1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>称重标签2</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -959,7 +936,82 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -968,12 +1020,67 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
-      <family val="3"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -982,7 +1089,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79992065187536243"/>
+        <fgColor theme="4" tint="0.799951170384838"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1006,7 +1113,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor theme="0" tint="-0.0499893185216834"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1018,12 +1125,198 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -1253,13 +1546,300 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1344,69 +1924,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1416,26 +1933,131 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <mruColors>
-      <color rgb="FFFF0000"/>
-      <color rgb="FFFFFF00"/>
+      <color rgb="00FF0000"/>
+      <color rgb="00FFFF00"/>
     </mruColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1723,14 +2345,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E70"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="8.75" customWidth="1"/>
     <col min="2" max="2" width="29.75" customWidth="1"/>
@@ -1739,51 +2362,51 @@
     <col min="5" max="5" width="101.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="49" t="s">
+    <row r="1" ht="19.5" spans="1:5">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="51"/>
-    </row>
-    <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="30"/>
+    </row>
+    <row r="2" ht="14.25"/>
+    <row r="3" ht="14.25" spans="1:5">
+      <c r="A3" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="33" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="28">
+    <row r="4" spans="1:5">
+      <c r="A4" s="34">
         <v>1</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="31" t="s">
+      <c r="C4" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="38" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5">
       <c r="A5" s="18">
         <v>2</v>
       </c>
@@ -1793,14 +2416,14 @@
       <c r="C5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="39" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5">
       <c r="A6" s="18">
         <v>3</v>
       </c>
@@ -1810,14 +2433,14 @@
       <c r="C6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="39" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5">
       <c r="A7" s="18">
         <v>4</v>
       </c>
@@ -1827,14 +2450,14 @@
       <c r="C7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="39" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5">
       <c r="A8" s="18">
         <v>5</v>
       </c>
@@ -1844,14 +2467,14 @@
       <c r="C8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="39" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5">
       <c r="A9" s="18">
         <v>6</v>
       </c>
@@ -1861,14 +2484,14 @@
       <c r="C9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="39" t="s">
         <v>19</v>
       </c>
       <c r="E9" s="20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5">
       <c r="A10" s="18">
         <v>7</v>
       </c>
@@ -1878,14 +2501,14 @@
       <c r="C10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="33" t="s">
+      <c r="D10" s="39" t="s">
         <v>21</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5">
       <c r="A11" s="18">
         <v>8</v>
       </c>
@@ -1895,14 +2518,14 @@
       <c r="C11" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="39" t="s">
         <v>23</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5">
       <c r="A12" s="18">
         <v>9</v>
       </c>
@@ -1912,14 +2535,14 @@
       <c r="C12" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="33" t="s">
+      <c r="D12" s="39" t="s">
         <v>25</v>
       </c>
       <c r="E12" s="20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5">
       <c r="A13" s="18">
         <v>10</v>
       </c>
@@ -1929,14 +2552,14 @@
       <c r="C13" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="33" t="s">
+      <c r="D13" s="39" t="s">
         <v>27</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5">
       <c r="A14" s="18">
         <v>11</v>
       </c>
@@ -1946,31 +2569,31 @@
       <c r="C14" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="33" t="s">
+      <c r="D14" s="39" t="s">
         <v>29</v>
       </c>
       <c r="E14" s="20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5">
       <c r="A15" s="18">
         <v>12</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>294</v>
+        <v>30</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="D15" s="40" t="s">
         <v>32</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5">
       <c r="A16" s="18">
         <v>13</v>
       </c>
@@ -1987,7 +2610,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5">
       <c r="A17" s="18">
         <v>14</v>
       </c>
@@ -2004,7 +2627,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5">
       <c r="A18" s="18">
         <v>15</v>
       </c>
@@ -2021,7 +2644,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5">
       <c r="A19" s="18">
         <v>16</v>
       </c>
@@ -2038,7 +2661,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5">
       <c r="A20" s="18">
         <v>17</v>
       </c>
@@ -2055,7 +2678,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5">
       <c r="A21" s="18">
         <v>18</v>
       </c>
@@ -2072,7 +2695,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5">
       <c r="A22" s="18">
         <v>19</v>
       </c>
@@ -2089,7 +2712,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5">
       <c r="A23" s="18">
         <v>20</v>
       </c>
@@ -2106,7 +2729,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5">
       <c r="A24" s="18">
         <v>21</v>
       </c>
@@ -2123,7 +2746,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5">
       <c r="A25" s="18">
         <v>22</v>
       </c>
@@ -2140,7 +2763,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5">
       <c r="A26" s="18">
         <v>23</v>
       </c>
@@ -2157,7 +2780,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5">
       <c r="A27" s="18">
         <v>24</v>
       </c>
@@ -2174,7 +2797,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5">
       <c r="A28" s="18">
         <v>25</v>
       </c>
@@ -2191,7 +2814,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5">
       <c r="A29" s="18">
         <v>26</v>
       </c>
@@ -2208,7 +2831,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5">
       <c r="A30" s="18">
         <v>27</v>
       </c>
@@ -2225,7 +2848,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5">
       <c r="A31" s="18">
         <v>28</v>
       </c>
@@ -2242,7 +2865,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5">
       <c r="A32" s="18">
         <v>29</v>
       </c>
@@ -2259,7 +2882,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5">
       <c r="A33" s="18">
         <v>30</v>
       </c>
@@ -2276,7 +2899,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5">
       <c r="A34" s="18">
         <v>31</v>
       </c>
@@ -2293,7 +2916,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5">
       <c r="A35" s="18">
         <v>32</v>
       </c>
@@ -2310,7 +2933,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5">
       <c r="A36" s="18">
         <v>33</v>
       </c>
@@ -2327,7 +2950,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5">
       <c r="A37" s="18">
         <v>34</v>
       </c>
@@ -2344,7 +2967,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5">
       <c r="A38" s="18">
         <v>35</v>
       </c>
@@ -2361,7 +2984,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5">
       <c r="A39" s="18">
         <v>36</v>
       </c>
@@ -2378,7 +3001,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5">
       <c r="A40" s="18">
         <v>37</v>
       </c>
@@ -2395,7 +3018,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5">
       <c r="A41" s="18">
         <v>38</v>
       </c>
@@ -2412,7 +3035,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5">
       <c r="A42" s="18">
         <v>39</v>
       </c>
@@ -2429,7 +3052,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5">
       <c r="A43" s="18">
         <v>40</v>
       </c>
@@ -2446,7 +3069,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:5">
       <c r="A44" s="18">
         <v>41</v>
       </c>
@@ -2463,7 +3086,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:5">
       <c r="A45" s="18">
         <v>42</v>
       </c>
@@ -2480,7 +3103,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:5">
       <c r="A46" s="18">
         <v>43</v>
       </c>
@@ -2497,7 +3120,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:5">
       <c r="A47" s="18">
         <v>44</v>
       </c>
@@ -2514,144 +3137,144 @@
         <v>78</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:5">
       <c r="A48" s="18">
         <v>45</v>
       </c>
       <c r="B48" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="C48" s="35" t="s">
+      <c r="C48" s="41" t="s">
         <v>100</v>
       </c>
-      <c r="D48" s="33" t="s">
+      <c r="D48" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="E48" s="36" t="s">
+      <c r="E48" s="42" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:5">
       <c r="A49" s="18">
         <v>46</v>
       </c>
-      <c r="B49" s="37" t="s">
+      <c r="B49" s="43" t="s">
         <v>103</v>
       </c>
       <c r="C49" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D49" s="33" t="s">
+      <c r="D49" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="E49" s="36" t="s">
+      <c r="E49" s="42" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:5">
       <c r="A50" s="18">
         <v>47</v>
       </c>
-      <c r="B50" s="37" t="s">
+      <c r="B50" s="43" t="s">
         <v>105</v>
       </c>
       <c r="C50" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D50" s="33" t="s">
+      <c r="D50" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="E50" s="36" t="s">
+      <c r="E50" s="42" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:5">
       <c r="A51" s="18">
         <v>48</v>
       </c>
-      <c r="B51" s="37" t="s">
+      <c r="B51" s="43" t="s">
         <v>107</v>
       </c>
       <c r="C51" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D51" s="33" t="s">
+      <c r="D51" s="39" t="s">
         <v>101</v>
       </c>
       <c r="E51" s="16" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:5">
       <c r="A52" s="18">
         <v>49</v>
       </c>
       <c r="B52" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="C52" s="35" t="s">
+      <c r="C52" s="41" t="s">
         <v>100</v>
       </c>
-      <c r="D52" s="34" t="s">
+      <c r="D52" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="E52" s="38" t="s">
+      <c r="E52" s="44" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:5">
       <c r="A53" s="18">
         <v>50</v>
       </c>
-      <c r="B53" s="37" t="s">
+      <c r="B53" s="43" t="s">
         <v>111</v>
       </c>
       <c r="C53" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D53" s="34" t="s">
+      <c r="D53" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="E53" s="38" t="s">
+      <c r="E53" s="44" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:5">
       <c r="A54" s="18">
         <v>51</v>
       </c>
-      <c r="B54" s="37" t="s">
+      <c r="B54" s="43" t="s">
         <v>113</v>
       </c>
       <c r="C54" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D54" s="34" t="s">
+      <c r="D54" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="E54" s="38" t="s">
+      <c r="E54" s="44" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:5">
       <c r="A55" s="18">
         <v>52</v>
       </c>
       <c r="B55" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="C55" s="35" t="s">
+      <c r="C55" s="41" t="s">
         <v>100</v>
       </c>
-      <c r="D55" s="33" t="s">
+      <c r="D55" s="39" t="s">
         <v>116</v>
       </c>
       <c r="E55" s="16" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A56" s="39">
+    <row r="56" spans="1:5">
+      <c r="A56" s="45">
         <v>53</v>
       </c>
       <c r="B56" s="27" t="s">
@@ -2660,32 +3283,32 @@
       <c r="C56" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="D56" s="40" t="s">
+      <c r="D56" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="E56" s="41" t="s">
+      <c r="E56" s="47" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A57" s="39">
+    <row r="57" spans="1:5">
+      <c r="A57" s="45">
         <v>55</v>
       </c>
-      <c r="B57" s="42" t="s">
+      <c r="B57" s="48" t="s">
         <v>119</v>
       </c>
-      <c r="C57" s="42" t="s">
+      <c r="C57" s="48" t="s">
         <v>120</v>
       </c>
-      <c r="D57" s="42" t="s">
+      <c r="D57" s="48" t="s">
         <v>121</v>
       </c>
-      <c r="E57" s="43" t="s">
+      <c r="E57" s="49" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A58" s="39">
+    <row r="58" spans="1:5">
+      <c r="A58" s="45">
         <v>56</v>
       </c>
       <c r="B58" s="27" t="s">
@@ -2697,12 +3320,12 @@
       <c r="D58" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="E58" s="41" t="s">
+      <c r="E58" s="47" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A59" s="39">
+    <row r="59" spans="1:5">
+      <c r="A59" s="45">
         <v>57</v>
       </c>
       <c r="B59" s="27" t="s">
@@ -2714,12 +3337,12 @@
       <c r="D59" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="E59" s="41" t="s">
+      <c r="E59" s="47" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A60" s="39">
+    <row r="60" spans="1:5">
+      <c r="A60" s="45">
         <v>58</v>
       </c>
       <c r="B60" s="27" t="s">
@@ -2731,12 +3354,12 @@
       <c r="D60" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="E60" s="41" t="s">
+      <c r="E60" s="47" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A61" s="39">
+    <row r="61" spans="1:5">
+      <c r="A61" s="45">
         <v>59</v>
       </c>
       <c r="B61" s="27" t="s">
@@ -2748,12 +3371,12 @@
       <c r="D61" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="E61" s="41" t="s">
+      <c r="E61" s="47" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A62" s="39">
+    <row r="62" spans="1:5">
+      <c r="A62" s="45">
         <v>60</v>
       </c>
       <c r="B62" s="27" t="s">
@@ -2765,12 +3388,12 @@
       <c r="D62" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="E62" s="41" t="s">
+      <c r="E62" s="47" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A63" s="39">
+    <row r="63" spans="1:5">
+      <c r="A63" s="45">
         <v>61</v>
       </c>
       <c r="B63" s="27" t="s">
@@ -2782,12 +3405,12 @@
       <c r="D63" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="E63" s="41" t="s">
+      <c r="E63" s="47" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A64" s="39">
+    <row r="64" spans="1:5">
+      <c r="A64" s="45">
         <v>62</v>
       </c>
       <c r="B64" s="27" t="s">
@@ -2799,12 +3422,12 @@
       <c r="D64" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="E64" s="41" t="s">
+      <c r="E64" s="47" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A65" s="39">
+    <row r="65" spans="1:5">
+      <c r="A65" s="45">
         <v>63</v>
       </c>
       <c r="B65" s="27" t="s">
@@ -2816,12 +3439,12 @@
       <c r="D65" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="E65" s="41" t="s">
+      <c r="E65" s="47" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A66" s="39">
+    <row r="66" spans="1:5">
+      <c r="A66" s="45">
         <v>64</v>
       </c>
       <c r="B66" s="27" t="s">
@@ -2833,12 +3456,12 @@
       <c r="D66" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="E66" s="41" t="s">
+      <c r="E66" s="47" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A67" s="39">
+    <row r="67" spans="1:5">
+      <c r="A67" s="45">
         <v>65</v>
       </c>
       <c r="B67" s="27" t="s">
@@ -2850,12 +3473,12 @@
       <c r="D67" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="E67" s="41" t="s">
+      <c r="E67" s="47" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A68" s="39">
+    <row r="68" spans="1:5">
+      <c r="A68" s="45">
         <v>66</v>
       </c>
       <c r="B68" s="27" t="s">
@@ -2867,63 +3490,37 @@
       <c r="D68" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="E68" s="41" t="s">
+      <c r="E68" s="47" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A69" s="39">
-        <v>67</v>
-      </c>
-      <c r="B69" s="19" t="s">
-        <v>169</v>
-      </c>
-      <c r="C69" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D69" s="19" t="s">
-        <v>297</v>
-      </c>
-      <c r="E69" s="20" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="48">
-        <v>68</v>
-      </c>
-      <c r="B70" s="44" t="s">
-        <v>171</v>
-      </c>
-      <c r="C70" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="D70" s="44" t="s">
-        <v>296</v>
-      </c>
-      <c r="E70" s="45" t="s">
-        <v>299</v>
-      </c>
+    <row r="69" ht="14.25" spans="1:5">
+      <c r="A69" s="50"/>
+      <c r="B69" s="51"/>
+      <c r="C69" s="51"/>
+      <c r="D69" s="51"/>
+      <c r="E69" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E156"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:E156"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="E109" sqref="B107:E109"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="E59" sqref="B49:E59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="4.875" customWidth="1"/>
     <col min="2" max="2" width="30.375" customWidth="1"/>
@@ -2932,7 +3529,8 @@
     <col min="5" max="5" width="65.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" ht="14.25"/>
+    <row r="2" ht="14.25" spans="1:5">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2949,7 +3547,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" s="1" customFormat="1" spans="1:5">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -2966,7 +3564,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" s="1" customFormat="1" spans="1:5">
       <c r="A4" s="11">
         <v>2</v>
       </c>
@@ -2983,7 +3581,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" s="1" customFormat="1" spans="1:5">
       <c r="A5" s="11">
         <v>3</v>
       </c>
@@ -3000,7 +3598,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" s="1" customFormat="1" spans="1:5">
       <c r="A6" s="11">
         <v>4</v>
       </c>
@@ -3017,7 +3615,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="7" s="1" customFormat="1" spans="1:5">
       <c r="A7" s="11">
         <v>5</v>
       </c>
@@ -3034,7 +3632,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="8" s="1" customFormat="1" spans="1:5">
       <c r="A8" s="11">
         <v>6</v>
       </c>
@@ -3051,7 +3649,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" s="1" customFormat="1" spans="1:5">
       <c r="A9" s="11">
         <v>7</v>
       </c>
@@ -3068,7 +3666,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="10" s="1" customFormat="1" spans="1:5">
       <c r="A10" s="11">
         <v>8</v>
       </c>
@@ -3085,7 +3683,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="11" s="2" customFormat="1" spans="1:5">
       <c r="A11" s="14">
         <v>10</v>
       </c>
@@ -3102,7 +3700,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="12" s="1" customFormat="1" spans="1:5">
       <c r="A12" s="11">
         <v>12</v>
       </c>
@@ -3119,7 +3717,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="13" s="1" customFormat="1" spans="1:5">
       <c r="A13" s="11">
         <v>13</v>
       </c>
@@ -3136,7 +3734,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" s="1" customFormat="1" spans="1:5">
       <c r="A14" s="11">
         <v>14</v>
       </c>
@@ -3153,7 +3751,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="15" s="1" customFormat="1" spans="1:5">
       <c r="A15" s="11">
         <v>15</v>
       </c>
@@ -3170,7 +3768,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="16" s="1" customFormat="1" spans="1:5">
       <c r="A16" s="11">
         <v>16</v>
       </c>
@@ -3187,7 +3785,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="17" s="1" customFormat="1" spans="1:5">
       <c r="A17" s="11">
         <v>17</v>
       </c>
@@ -3204,7 +3802,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" s="1" customFormat="1" spans="1:5">
       <c r="A18" s="11">
         <v>18</v>
       </c>
@@ -3221,7 +3819,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5">
       <c r="A19" s="18">
         <v>20</v>
       </c>
@@ -3238,7 +3836,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5">
       <c r="A20" s="18">
         <v>21</v>
       </c>
@@ -3255,7 +3853,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5">
       <c r="A21" s="18">
         <v>22</v>
       </c>
@@ -3272,7 +3870,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="22" s="1" customFormat="1" spans="1:5">
       <c r="A22" s="11">
         <v>24</v>
       </c>
@@ -3289,7 +3887,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="23" s="1" customFormat="1" spans="1:5">
       <c r="A23" s="11">
         <v>25</v>
       </c>
@@ -3306,7 +3904,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="24" s="1" customFormat="1" spans="1:5">
       <c r="A24" s="11">
         <v>26</v>
       </c>
@@ -3323,7 +3921,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5">
       <c r="A25" s="18">
         <v>28</v>
       </c>
@@ -3340,7 +3938,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5">
       <c r="A26" s="18">
         <v>29</v>
       </c>
@@ -3357,7 +3955,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="27" s="1" customFormat="1" spans="1:5">
       <c r="A27" s="11">
         <v>31</v>
       </c>
@@ -3374,7 +3972,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="28" s="1" customFormat="1" spans="1:5">
       <c r="A28" s="11">
         <v>32</v>
       </c>
@@ -3391,7 +3989,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="29" s="1" customFormat="1" spans="1:5">
       <c r="A29" s="11">
         <v>33</v>
       </c>
@@ -3408,7 +4006,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="30" s="1" customFormat="1" spans="1:5">
       <c r="A30" s="11">
         <v>34</v>
       </c>
@@ -3425,7 +4023,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="31" s="1" customFormat="1" spans="1:5">
       <c r="A31" s="11">
         <v>35</v>
       </c>
@@ -3442,7 +4040,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="32" s="1" customFormat="1" spans="1:5">
       <c r="A32" s="11">
         <v>36</v>
       </c>
@@ -3459,7 +4057,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="33" s="1" customFormat="1" spans="1:5">
       <c r="A33" s="11">
         <v>37</v>
       </c>
@@ -3476,7 +4074,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="34" s="1" customFormat="1" spans="1:5">
       <c r="A34" s="11">
         <v>38</v>
       </c>
@@ -3493,7 +4091,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="35" s="1" customFormat="1" spans="1:5">
       <c r="A35" s="11">
         <v>39</v>
       </c>
@@ -3510,7 +4108,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="36" s="1" customFormat="1" spans="1:5">
       <c r="A36" s="11">
         <v>40</v>
       </c>
@@ -3527,7 +4125,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="37" s="1" customFormat="1" spans="1:5">
       <c r="A37" s="11">
         <v>41</v>
       </c>
@@ -3544,7 +4142,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5">
       <c r="A38" s="18">
         <v>43</v>
       </c>
@@ -3561,7 +4159,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5">
       <c r="A39" s="18">
         <v>44</v>
       </c>
@@ -3578,7 +4176,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5">
       <c r="A40" s="18">
         <v>45</v>
       </c>
@@ -3595,7 +4193,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5">
       <c r="A41" s="18">
         <v>46</v>
       </c>
@@ -3612,7 +4210,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5">
       <c r="A42" s="18">
         <v>47</v>
       </c>
@@ -3629,7 +4227,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5">
       <c r="A43" s="18">
         <v>48</v>
       </c>
@@ -3646,7 +4244,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:5">
       <c r="A44" s="18">
         <v>49</v>
       </c>
@@ -3663,7 +4261,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:5">
       <c r="A45" s="18">
         <v>50</v>
       </c>
@@ -3680,7 +4278,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:5">
       <c r="A46" s="18">
         <v>51</v>
       </c>
@@ -3697,7 +4295,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:5">
       <c r="A47" s="18">
         <v>52</v>
       </c>
@@ -3714,7 +4312,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:5">
       <c r="A48" s="18">
         <v>53</v>
       </c>
@@ -3731,7 +4329,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="49" s="1" customFormat="1" spans="1:5">
       <c r="A49" s="11">
         <v>55</v>
       </c>
@@ -3748,7 +4346,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="50" s="1" customFormat="1" spans="1:5">
       <c r="A50" s="11">
         <v>56</v>
       </c>
@@ -3765,7 +4363,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="51" s="1" customFormat="1" spans="1:5">
       <c r="A51" s="11">
         <v>57</v>
       </c>
@@ -3782,7 +4380,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="52" s="1" customFormat="1" spans="1:5">
       <c r="A52" s="11">
         <v>58</v>
       </c>
@@ -3799,7 +4397,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="53" s="1" customFormat="1" spans="1:5">
       <c r="A53" s="11">
         <v>59</v>
       </c>
@@ -3816,7 +4414,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="54" s="1" customFormat="1" spans="1:5">
       <c r="A54" s="11">
         <v>60</v>
       </c>
@@ -3833,7 +4431,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="55" s="1" customFormat="1" spans="1:5">
       <c r="A55" s="11">
         <v>61</v>
       </c>
@@ -3850,7 +4448,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="56" s="1" customFormat="1" spans="1:5">
       <c r="A56" s="11">
         <v>62</v>
       </c>
@@ -3867,7 +4465,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="57" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="57" s="1" customFormat="1" spans="1:5">
       <c r="A57" s="11">
         <v>63</v>
       </c>
@@ -3884,7 +4482,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="58" s="1" customFormat="1" spans="1:5">
       <c r="A58" s="11">
         <v>64</v>
       </c>
@@ -3901,7 +4499,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="59" s="1" customFormat="1" spans="1:5">
       <c r="A59" s="11">
         <v>65</v>
       </c>
@@ -3918,7 +4516,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:5">
       <c r="A60" s="18">
         <v>68</v>
       </c>
@@ -3935,7 +4533,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:5">
       <c r="A61" s="18">
         <v>69</v>
       </c>
@@ -3952,7 +4550,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:5">
       <c r="A62" s="18">
         <v>70</v>
       </c>
@@ -3969,7 +4567,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="63" s="1" customFormat="1" spans="1:5">
       <c r="A63" s="11">
         <v>72</v>
       </c>
@@ -3986,7 +4584,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="64" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="64" s="1" customFormat="1" spans="1:5">
       <c r="A64" s="11">
         <v>73</v>
       </c>
@@ -4003,7 +4601,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="65" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="65" s="1" customFormat="1" spans="1:5">
       <c r="A65" s="11">
         <v>74</v>
       </c>
@@ -4020,7 +4618,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:5">
       <c r="A66" s="18">
         <v>76</v>
       </c>
@@ -4037,7 +4635,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:5">
       <c r="A67" s="18">
         <v>77</v>
       </c>
@@ -4054,7 +4652,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:5">
       <c r="A68" s="18">
         <v>78</v>
       </c>
@@ -4071,7 +4669,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="69" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="69" s="1" customFormat="1" spans="1:5">
       <c r="A69" s="11">
         <v>80</v>
       </c>
@@ -4088,7 +4686,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="70" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="70" s="1" customFormat="1" spans="1:5">
       <c r="A70" s="11">
         <v>81</v>
       </c>
@@ -4105,7 +4703,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="71" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="71" s="1" customFormat="1" spans="1:5">
       <c r="A71" s="11">
         <v>82</v>
       </c>
@@ -4122,7 +4720,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:5">
       <c r="A72" s="18">
         <v>84</v>
       </c>
@@ -4139,7 +4737,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:5">
       <c r="A73" s="18">
         <v>85</v>
       </c>
@@ -4156,7 +4754,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:5">
       <c r="A74" s="18">
         <v>86</v>
       </c>
@@ -4173,7 +4771,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="75" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="75" s="1" customFormat="1" spans="1:5">
       <c r="A75" s="11">
         <v>88</v>
       </c>
@@ -4190,7 +4788,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="76" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="76" s="1" customFormat="1" spans="1:5">
       <c r="A76" s="11">
         <v>89</v>
       </c>
@@ -4207,7 +4805,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="77" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="77" s="1" customFormat="1" spans="1:5">
       <c r="A77" s="11">
         <v>90</v>
       </c>
@@ -4224,7 +4822,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:5">
       <c r="A78" s="18">
         <v>92</v>
       </c>
@@ -4241,7 +4839,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:5">
       <c r="A79" s="18">
         <v>93</v>
       </c>
@@ -4258,7 +4856,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:5">
       <c r="A80" s="18">
         <v>94</v>
       </c>
@@ -4275,7 +4873,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="81" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="81" s="1" customFormat="1" spans="1:5">
       <c r="A81" s="11">
         <v>96</v>
       </c>
@@ -4292,7 +4890,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="82" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="82" s="1" customFormat="1" spans="1:5">
       <c r="A82" s="11">
         <v>97</v>
       </c>
@@ -4309,7 +4907,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="83" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="83" s="1" customFormat="1" spans="1:5">
       <c r="A83" s="11">
         <v>98</v>
       </c>
@@ -4326,7 +4924,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:5">
       <c r="A84" s="18">
         <v>100</v>
       </c>
@@ -4343,7 +4941,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:5">
       <c r="A85" s="18">
         <v>101</v>
       </c>
@@ -4360,7 +4958,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:5">
       <c r="A86" s="18">
         <v>102</v>
       </c>
@@ -4377,7 +4975,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="87" spans="1:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="87" s="1" customFormat="1" ht="18" customHeight="1" spans="1:5">
       <c r="A87" s="11">
         <v>104</v>
       </c>
@@ -4394,7 +4992,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="88" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="88" s="1" customFormat="1" spans="1:5">
       <c r="A88" s="11">
         <v>105</v>
       </c>
@@ -4411,7 +5009,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="89" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="89" s="1" customFormat="1" spans="1:5">
       <c r="A89" s="11">
         <v>106</v>
       </c>
@@ -4428,7 +5026,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:5">
       <c r="A90" s="18">
         <v>108</v>
       </c>
@@ -4445,7 +5043,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:5">
       <c r="A91" s="18">
         <v>109</v>
       </c>
@@ -4462,7 +5060,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:5">
       <c r="A92" s="18">
         <v>110</v>
       </c>
@@ -4479,7 +5077,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="93" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="93" s="1" customFormat="1" spans="1:5">
       <c r="A93" s="11">
         <v>112</v>
       </c>
@@ -4496,7 +5094,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="94" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="94" s="1" customFormat="1" spans="1:5">
       <c r="A94" s="11">
         <v>113</v>
       </c>
@@ -4513,7 +5111,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="95" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="95" s="1" customFormat="1" spans="1:5">
       <c r="A95" s="11">
         <v>114</v>
       </c>
@@ -4530,7 +5128,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:5">
       <c r="A96" s="18">
         <v>116</v>
       </c>
@@ -4547,7 +5145,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:5">
       <c r="A97" s="18">
         <v>117</v>
       </c>
@@ -4564,7 +5162,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:5">
       <c r="A98" s="18">
         <v>118</v>
       </c>
@@ -4581,7 +5179,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="99" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="99" s="1" customFormat="1" spans="1:5">
       <c r="A99" s="11">
         <v>120</v>
       </c>
@@ -4598,7 +5196,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="100" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="100" s="1" customFormat="1" spans="1:5">
       <c r="A100" s="11">
         <v>121</v>
       </c>
@@ -4615,7 +5213,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="101" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="101" s="1" customFormat="1" spans="1:5">
       <c r="A101" s="11">
         <v>122</v>
       </c>
@@ -4632,7 +5230,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="102" ht="15.95" customHeight="1" spans="1:5">
       <c r="A102" s="18">
         <v>124</v>
       </c>
@@ -4649,7 +5247,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:5">
       <c r="A103" s="18">
         <v>125</v>
       </c>
@@ -4666,7 +5264,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:5">
       <c r="A104" s="18">
         <v>126</v>
       </c>
@@ -4683,7 +5281,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="105" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="105" s="1" customFormat="1" ht="14.25" spans="1:5">
       <c r="A105" s="23">
         <v>131</v>
       </c>
@@ -4700,7 +5298,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="106" spans="2:5">
       <c r="B106" s="12" t="s">
         <v>262</v>
       </c>
@@ -4714,49 +5312,40 @@
         <v>264</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B107" s="46" t="s">
+    <row r="107" spans="2:4">
+      <c r="B107" s="12" t="s">
         <v>265</v>
       </c>
-      <c r="C107" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="D107" s="47" t="s">
+      <c r="C107" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D107" t="s">
         <v>266</v>
       </c>
-      <c r="E107" s="47" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B108" s="46" t="s">
+    </row>
+    <row r="108" spans="2:4">
+      <c r="B108" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="C108" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="D108" s="47" t="s">
+      <c r="C108" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D108" t="s">
         <v>268</v>
       </c>
-      <c r="E108" s="47" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B109" s="46" t="s">
+    </row>
+    <row r="109" spans="2:4">
+      <c r="B109" s="12" t="s">
         <v>269</v>
       </c>
-      <c r="C109" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="D109" s="47" t="s">
+      <c r="C109" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D109" t="s">
         <v>270</v>
       </c>
-      <c r="E109" s="47" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="110" spans="2:4">
       <c r="B110" s="26" t="s">
         <v>271</v>
       </c>
@@ -4767,7 +5356,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="111" spans="2:4">
       <c r="B111" s="26" t="s">
         <v>273</v>
       </c>
@@ -4778,7 +5367,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="112" spans="2:4">
       <c r="B112" s="26" t="s">
         <v>275</v>
       </c>
@@ -4789,7 +5378,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="116" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="116" spans="2:4">
       <c r="B116" s="27" t="s">
         <v>277</v>
       </c>
@@ -4800,7 +5389,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="117" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="117" spans="2:4">
       <c r="B117" s="27" t="s">
         <v>279</v>
       </c>
@@ -4811,7 +5400,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="118" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="118" spans="2:4">
       <c r="B118" s="27" t="s">
         <v>280</v>
       </c>
@@ -4822,7 +5411,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="120" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="120" spans="2:5">
       <c r="B120" s="27" t="s">
         <v>6</v>
       </c>
@@ -4836,7 +5425,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="121" spans="2:5">
       <c r="B121" s="27" t="s">
         <v>10</v>
       </c>
@@ -4850,7 +5439,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="123" spans="2:5">
       <c r="B123" s="27" t="s">
         <v>12</v>
       </c>
@@ -4864,7 +5453,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="124" spans="2:5">
       <c r="B124" s="27" t="s">
         <v>14</v>
       </c>
@@ -4878,7 +5467,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="125" spans="2:5">
       <c r="B125" s="27" t="s">
         <v>16</v>
       </c>
@@ -4892,7 +5481,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="126" spans="2:5">
       <c r="B126" s="27" t="s">
         <v>18</v>
       </c>
@@ -4906,7 +5495,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="127" spans="2:5">
       <c r="B127" s="27" t="s">
         <v>20</v>
       </c>
@@ -4920,7 +5509,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="129" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="129" spans="2:5">
       <c r="B129" s="27" t="s">
         <v>22</v>
       </c>
@@ -4934,7 +5523,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="130" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="130" spans="2:5">
       <c r="B130" s="27" t="s">
         <v>24</v>
       </c>
@@ -4948,7 +5537,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="131" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="131" spans="2:5">
       <c r="B131" s="27" t="s">
         <v>26</v>
       </c>
@@ -4962,7 +5551,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="132" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="132" spans="2:5">
       <c r="B132" s="27" t="s">
         <v>28</v>
       </c>
@@ -4976,7 +5565,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="135" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="135" spans="2:5">
       <c r="B135" s="27" t="s">
         <v>281</v>
       </c>
@@ -4990,7 +5579,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="136" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="136" spans="2:4">
       <c r="B136" s="27" t="s">
         <v>123</v>
       </c>
@@ -5001,7 +5590,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="137" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="137" spans="2:4">
       <c r="B137" s="27" t="s">
         <v>126</v>
       </c>
@@ -5012,7 +5601,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="138" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="138" spans="2:4">
       <c r="B138" s="27" t="s">
         <v>128</v>
       </c>
@@ -5023,7 +5612,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="139" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="139" spans="2:4">
       <c r="B139" s="27" t="s">
         <v>130</v>
       </c>
@@ -5034,7 +5623,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="140" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="140" spans="2:4">
       <c r="B140" s="27" t="s">
         <v>132</v>
       </c>
@@ -5045,7 +5634,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="141" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="141" spans="2:4">
       <c r="B141" s="27" t="s">
         <v>134</v>
       </c>
@@ -5056,7 +5645,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="142" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="142" spans="2:4">
       <c r="B142" s="27" t="s">
         <v>136</v>
       </c>
@@ -5067,7 +5656,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="143" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="143" spans="2:4">
       <c r="B143" s="27" t="s">
         <v>138</v>
       </c>
@@ -5078,7 +5667,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="144" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="144" spans="2:4">
       <c r="B144" s="27" t="s">
         <v>140</v>
       </c>
@@ -5089,7 +5678,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="145" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="145" spans="2:4">
       <c r="B145" s="27" t="s">
         <v>142</v>
       </c>
@@ -5100,7 +5689,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="146" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="146" spans="2:4">
       <c r="B146" s="27" t="s">
         <v>144</v>
       </c>
@@ -5111,7 +5700,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="147" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="147" spans="2:4">
       <c r="B147" s="27" t="s">
         <v>284</v>
       </c>
@@ -5122,7 +5711,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="148" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="148" spans="2:4">
       <c r="B148" s="27" t="s">
         <v>285</v>
       </c>
@@ -5133,7 +5722,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="149" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="149" spans="2:4">
       <c r="B149" s="27" t="s">
         <v>286</v>
       </c>
@@ -5144,7 +5733,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="150" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="150" spans="2:4">
       <c r="B150" s="27" t="s">
         <v>287</v>
       </c>
@@ -5155,7 +5744,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="151" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="151" spans="2:4">
       <c r="B151" s="27" t="s">
         <v>288</v>
       </c>
@@ -5166,7 +5755,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="152" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="152" spans="2:4">
       <c r="B152" s="27" t="s">
         <v>289</v>
       </c>
@@ -5177,7 +5766,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="153" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="153" spans="2:4">
       <c r="B153" s="27" t="s">
         <v>290</v>
       </c>
@@ -5188,7 +5777,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="154" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="154" spans="2:4">
       <c r="B154" s="27" t="s">
         <v>291</v>
       </c>
@@ -5199,7 +5788,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="155" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="155" spans="2:4">
       <c r="B155" s="27" t="s">
         <v>292</v>
       </c>
@@ -5210,7 +5799,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="156" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="156" spans="2:4">
       <c r="B156" s="27" t="s">
         <v>293</v>
       </c>
@@ -5222,8 +5811,8 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>